<commit_message>
Change the form of xlsx file
</commit_message>
<xml_diff>
--- a/ucla_cse.xlsx
+++ b/ucla_cse.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11118"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steveli/Developer/Python/ECE143_Project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34EAA93-0771-CB4A-B1D3-6B11A99FFD47}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="11520" yWindow="2040" windowWidth="17280" windowHeight="18040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -430,12 +436,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -443,8 +449,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -490,15 +503,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -540,7 +561,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,9 +593,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,6 +645,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -781,12 +838,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="4" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
@@ -5952,6 +6015,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>